<commit_message>
Update PCB via size, start with code infrastructure idea
</commit_message>
<xml_diff>
--- a/hardware/OpenHand_v3/Datasheets/STM32_Pin_Assignment.xlsx
+++ b/hardware/OpenHand_v3/Datasheets/STM32_Pin_Assignment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="200">
   <si>
     <t xml:space="preserve">Pin #</t>
   </si>
@@ -361,13 +361,16 @@
     <t xml:space="preserve">ADC12_IN14</t>
   </si>
   <si>
-    <t xml:space="preserve">testpoint (ADC)</t>
+    <t xml:space="preserve">PCB_TEMP_01</t>
   </si>
   <si>
     <t xml:space="preserve">PC5</t>
   </si>
   <si>
     <t xml:space="preserve">ADC12_IN15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB_TEMP_02</t>
   </si>
   <si>
     <t xml:space="preserve">PB0</t>
@@ -1244,7 +1247,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="C2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1736,15 +1739,15 @@
         <v>78</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="6" t="s">
+      <c r="G25" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -1754,33 +1757,33 @@
         <v>81</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="6" t="s">
-        <v>80</v>
-      </c>
+      <c r="G26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H27" s="6"/>
     </row>
@@ -1789,18 +1792,18 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H28" s="6"/>
     </row>
@@ -1809,7 +1812,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>61</v>
@@ -1818,7 +1821,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H29" s="6"/>
     </row>
@@ -1827,20 +1830,20 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H30" s="6"/>
     </row>
@@ -1849,20 +1852,20 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H31" s="6"/>
     </row>
@@ -1907,18 +1910,18 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H34" s="6"/>
     </row>
@@ -1927,20 +1930,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H35" s="6"/>
     </row>
@@ -1949,20 +1952,20 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H36" s="6"/>
     </row>
@@ -1971,20 +1974,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H37" s="6"/>
     </row>
@@ -1993,16 +1996,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H38" s="6"/>
     </row>
@@ -2011,16 +2014,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H39" s="6"/>
     </row>
@@ -2029,16 +2032,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H40" s="6"/>
     </row>
@@ -2047,16 +2050,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H41" s="6"/>
     </row>
@@ -2065,18 +2068,18 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H42" s="6"/>
     </row>
@@ -2085,20 +2088,20 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H43" s="6"/>
     </row>
@@ -2107,20 +2110,20 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H44" s="6"/>
     </row>
@@ -2129,18 +2132,18 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H45" s="6"/>
     </row>
@@ -2149,18 +2152,18 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H46" s="6"/>
     </row>
@@ -2169,16 +2172,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H47" s="6"/>
     </row>
@@ -2223,16 +2226,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H50" s="6"/>
     </row>
@@ -2241,18 +2244,18 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H51" s="6"/>
     </row>
@@ -2261,16 +2264,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H52" s="6"/>
     </row>
@@ -2279,16 +2282,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H53" s="6"/>
     </row>
@@ -2297,7 +2300,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>61</v>
@@ -2305,10 +2308,10 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H54" s="6"/>
     </row>
@@ -2317,20 +2320,20 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H55" s="6"/>
     </row>
@@ -2339,19 +2342,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="9"/>
       <c r="E56" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,19 +2362,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="9"/>
       <c r="E57" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,19 +2382,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="9"/>
       <c r="E58" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,18 +2402,18 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H59" s="6"/>
     </row>
@@ -2419,18 +2422,18 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H60" s="6"/>
     </row>
@@ -2439,19 +2442,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,18 +2462,18 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H62" s="6"/>
     </row>
@@ -2479,18 +2482,18 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H63" s="6"/>
     </row>

</xml_diff>